<commit_message>
adding UA collaboration 2024 data
</commit_message>
<xml_diff>
--- a/collaborations/all_topics_sorted.xlsx
+++ b/collaborations/all_topics_sorted.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B461"/>
+  <dimension ref="A1:B475"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,7 +376,7 @@
         </is>
       </c>
       <c r="B2">
-        <v>306</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3">
@@ -386,7 +386,7 @@
         </is>
       </c>
       <c r="B3">
-        <v>166</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4">
@@ -396,273 +396,273 @@
         </is>
       </c>
       <c r="B4">
-        <v>151</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Physics and Astronomy</t>
+          <t>Life Sciences</t>
         </is>
       </c>
       <c r="B5">
-        <v>123</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Astronomy and Astrophysics</t>
+          <t>Physics and Astronomy</t>
         </is>
       </c>
       <c r="B6">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Engineering</t>
+          <t>Astronomy and Astrophysics</t>
         </is>
       </c>
       <c r="B7">
-        <v>77</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Social Sciences</t>
+          <t>Engineering</t>
         </is>
       </c>
       <c r="B8">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Life Sciences</t>
+          <t>Biochemistry, Genetics and Molecular Biology</t>
         </is>
       </c>
       <c r="B9">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Environmental Science</t>
+          <t>Social Sciences</t>
         </is>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Earth and Planetary Sciences</t>
+          <t>Computer Science</t>
         </is>
       </c>
       <c r="B11">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Biochemistry, Genetics and Molecular Biology</t>
+          <t>Environmental Science</t>
         </is>
       </c>
       <c r="B12">
-        <v>27</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Epidemiology</t>
+          <t>Agricultural and Biological Sciences</t>
         </is>
       </c>
       <c r="B13">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Surgery</t>
+          <t>Molecular Biology</t>
         </is>
       </c>
       <c r="B14">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Atmospheric Science</t>
+          <t>Earth and Planetary Sciences</t>
         </is>
       </c>
       <c r="B15">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mechanics of Materials</t>
+          <t>Surgery</t>
         </is>
       </c>
       <c r="B16">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Computer Science</t>
+          <t>Plant Science</t>
         </is>
       </c>
       <c r="B17">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Numerical methods in engineering</t>
+          <t>Atmospheric Science</t>
         </is>
       </c>
       <c r="B18">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Stellar, planetary, and galactic studies</t>
+          <t>Galaxies: Formation, Evolution, Phenomena</t>
         </is>
       </c>
       <c r="B19">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Galaxies: Formation, Evolution, Phenomena</t>
+          <t>Electrical and Electronic Engineering</t>
         </is>
       </c>
       <c r="B20">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Civil and Structural Engineering</t>
+          <t>Psychology</t>
         </is>
       </c>
       <c r="B21">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Electrical and Electronic Engineering</t>
+          <t>Chemistry</t>
         </is>
       </c>
       <c r="B22">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Gamma-ray bursts and supernovae</t>
+          <t>Neuroscience</t>
         </is>
       </c>
       <c r="B23">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Molecular Biology</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="B24">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Pulmonary and Respiratory Medicine</t>
+          <t>Biomedical Engineering</t>
         </is>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Astronomy and Astrophysical Research</t>
+          <t>Ecology</t>
         </is>
       </c>
       <c r="B26">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Cosmology and Gravitation Theories</t>
+          <t>Stellar, planetary, and galactic studies</t>
         </is>
       </c>
       <c r="B27">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Instrumentation</t>
+          <t>Cardiology and Cardiovascular Medicine</t>
         </is>
       </c>
       <c r="B28">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Geotechnical Engineering and Underground Structures</t>
+          <t>Astronomy and Astrophysical Research</t>
         </is>
       </c>
       <c r="B29">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Atomic and Molecular Physics, and Optics</t>
+          <t>Astrophysics and Star Formation Studies</t>
         </is>
       </c>
       <c r="B30">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Astro and Planetary Science</t>
+          <t>Ecology, Evolution, Behavior and Systematics</t>
         </is>
       </c>
       <c r="B31">
@@ -672,7 +672,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Biomedical Engineering</t>
+          <t>Genetics</t>
         </is>
       </c>
       <c r="B32">
@@ -682,7 +682,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Genetics</t>
+          <t>Instrumentation</t>
         </is>
       </c>
       <c r="B33">
@@ -692,7 +692,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Materials Science</t>
+          <t>Social Psychology</t>
         </is>
       </c>
       <c r="B34">
@@ -702,17 +702,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Nuclear and High Energy Physics</t>
+          <t>Epidemiology</t>
         </is>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Agricultural and Biological Sciences</t>
+          <t>Health Professions</t>
         </is>
       </c>
       <c r="B36">
@@ -722,7 +722,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Global and Planetary Change</t>
+          <t>Infectious Diseases</t>
         </is>
       </c>
       <c r="B37">
@@ -732,7 +732,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Health Professions</t>
+          <t>Mathematics</t>
         </is>
       </c>
       <c r="B38">
@@ -742,7 +742,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Oncology</t>
+          <t>Mechanics of Materials</t>
         </is>
       </c>
       <c r="B39">
@@ -752,27 +752,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Business, Management and Accounting</t>
+          <t>Neurology</t>
         </is>
       </c>
       <c r="B40">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Cardiology and Cardiovascular Medicine</t>
+          <t>Pulmonary and Respiratory Medicine</t>
         </is>
       </c>
       <c r="B41">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Electromagnetic Simulation and Numerical Methods</t>
+          <t>Aerospace Engineering</t>
         </is>
       </c>
       <c r="B42">
@@ -782,7 +782,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Infectious Diseases</t>
+          <t>Astro and Planetary Science</t>
         </is>
       </c>
       <c r="B43">
@@ -792,7 +792,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Materials Chemistry</t>
+          <t>Economics, Econometrics and Finance</t>
         </is>
       </c>
       <c r="B44">
@@ -802,37 +802,37 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
+          <t>Global and Planetary Change</t>
         </is>
       </c>
       <c r="B45">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Astrophysics and Star Formation Studies</t>
+          <t>Nuclear and High Energy Physics</t>
         </is>
       </c>
       <c r="B46">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Chemistry</t>
+          <t>Physiology</t>
         </is>
       </c>
       <c r="B47">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Computational Mechanics</t>
+          <t>Computer Networks and Communications</t>
         </is>
       </c>
       <c r="B48">
@@ -842,7 +842,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Cryospheric studies and observations</t>
+          <t>Organic Chemistry</t>
         </is>
       </c>
       <c r="B49">
@@ -852,131 +852,131 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Health, Toxicology and Mutagenesis</t>
+          <t>Cognitive Neuroscience</t>
         </is>
       </c>
       <c r="B50">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Material Properties and Failure Mechanisms</t>
+          <t>Cosmology and Gravitation Theories</t>
         </is>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Mathematics</t>
+          <t>Gamma-ray bursts and supernovae</t>
         </is>
       </c>
       <c r="B52">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Obstetrics and Gynecology</t>
+          <t>Health, Toxicology and Mutagenesis</t>
         </is>
       </c>
       <c r="B53">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Plant Science</t>
+          <t>Information Systems</t>
         </is>
       </c>
       <c r="B54">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Psychology</t>
+          <t>Atomic and Molecular Physics, and Optics</t>
         </is>
       </c>
       <c r="B55">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Radiology, Nuclear Medicine and Imaging</t>
+          <t>Computational Mechanics</t>
         </is>
       </c>
       <c r="B56">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Sociology and Political Science</t>
+          <t>Computational Theory and Mathematics</t>
         </is>
       </c>
       <c r="B57">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Atmospheric Ozone and Climate</t>
+          <t>Computer Vision and Pattern Recognition</t>
         </is>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Climate variability and models</t>
+          <t>EEG and Brain-Computer Interfaces</t>
         </is>
       </c>
       <c r="B59">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Computer Vision and Pattern Recognition</t>
+          <t>Economics and Econometrics</t>
         </is>
       </c>
       <c r="B60">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Ecology</t>
+          <t>Endocrinology, Diabetes and Metabolism</t>
         </is>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Economics, Econometrics and Finance</t>
+          <t>Gastroenterology</t>
         </is>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="B63">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="64">
@@ -996,33 +996,33 @@
         </is>
       </c>
       <c r="B64">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Pancreatitis Pathology and Treatment</t>
+          <t>Immunology and Microbiology</t>
         </is>
       </c>
       <c r="B65">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Pediatrics, Perinatology and Child Health</t>
+          <t>Light effects on plants</t>
         </is>
       </c>
       <c r="B66">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Adaptive optics and wavefront sensing</t>
+          <t>Mitochondrial Function and Pathology</t>
         </is>
       </c>
       <c r="B67">
@@ -1032,7 +1032,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Astrophysics and Cosmic Phenomena</t>
+          <t>Nursing</t>
         </is>
       </c>
       <c r="B68">
@@ -1042,7 +1042,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Computational Theory and Mathematics</t>
+          <t>Nutrition and Dietetics</t>
         </is>
       </c>
       <c r="B69">
@@ -1052,7 +1052,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Emergency Medicine</t>
+          <t>Oncology</t>
         </is>
       </c>
       <c r="B70">
@@ -1062,7 +1062,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Endometrial and Cervical Cancer Treatments</t>
+          <t>Radiology, Nuclear Medicine and Imaging</t>
         </is>
       </c>
       <c r="B71">
@@ -1072,7 +1072,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Geophysical Methods and Applications</t>
+          <t>Smart Agriculture and AI</t>
         </is>
       </c>
       <c r="B72">
@@ -1082,137 +1082,137 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Global Maternal and Child Health</t>
+          <t>AI in cancer detection</t>
         </is>
       </c>
       <c r="B73">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Head and Neck Cancer Studies</t>
+          <t>Air Quality and Health Impacts</t>
         </is>
       </c>
       <c r="B74">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Mechanical Engineering</t>
+          <t>Animal Behavior and Reproduction</t>
         </is>
       </c>
       <c r="B75">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Neurology</t>
+          <t>Arctic and Antarctic ice dynamics</t>
         </is>
       </c>
       <c r="B76">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Nursing</t>
+          <t>Artificial Intelligence in Healthcare</t>
         </is>
       </c>
       <c r="B77">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Nutrition and Dietetics</t>
+          <t>Astrophysics and Cosmic Phenomena</t>
         </is>
       </c>
       <c r="B78">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Ocean Engineering</t>
+          <t>Bariatric Surgery and Outcomes</t>
         </is>
       </c>
       <c r="B79">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Organic Chemistry</t>
+          <t>Cancer Research</t>
         </is>
       </c>
       <c r="B80">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Orthopedic Infections and Treatments</t>
+          <t>Cardiac, Anesthesia and Surgical Outcomes</t>
         </is>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Otorhinolaryngology</t>
+          <t>Circadian rhythm and melatonin</t>
         </is>
       </c>
       <c r="B82">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Physiology</t>
+          <t>Civil and Structural Engineering</t>
         </is>
       </c>
       <c r="B83">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Statistical and Nonlinear Physics</t>
+          <t>Climate variability and models</t>
         </is>
       </c>
       <c r="B84">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Winter Sports Injuries and Performance</t>
+          <t>Clinical Psychology</t>
         </is>
       </c>
       <c r="B85">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Accounting</t>
+          <t>Cryospheric studies and observations</t>
         </is>
       </c>
       <c r="B86">
@@ -1222,7 +1222,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Advanced Numerical Methods in Computational Mathematics</t>
+          <t>Endocrine and Autonomic Systems</t>
         </is>
       </c>
       <c r="B87">
@@ -1232,7 +1232,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Aerospace Engineering</t>
+          <t>Finance</t>
         </is>
       </c>
       <c r="B88">
@@ -1242,7 +1242,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Antifungal resistance and susceptibility</t>
+          <t>Health</t>
         </is>
       </c>
       <c r="B89">
@@ -1252,7 +1252,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Astrophysical Phenomena and Observations</t>
+          <t>Health Information Management</t>
         </is>
       </c>
       <c r="B90">
@@ -1262,7 +1262,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>COVID-19 Clinical Research Studies</t>
+          <t>Materials Science</t>
         </is>
       </c>
       <c r="B91">
@@ -1272,7 +1272,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>COVID-19 diagnosis using AI</t>
+          <t>Mathematical Physics</t>
         </is>
       </c>
       <c r="B92">
@@ -1282,7 +1282,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Cell Biology</t>
+          <t>Mechanical Engineering</t>
         </is>
       </c>
       <c r="B93">
@@ -1292,7 +1292,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Child Nutrition and Water Access</t>
+          <t>Nature and Landscape Conservation</t>
         </is>
       </c>
       <c r="B94">
@@ -1302,7 +1302,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Chronic Obstructive Pulmonary Disease (COPD) Research</t>
+          <t>Oceanography</t>
         </is>
       </c>
       <c r="B95">
@@ -1312,7 +1312,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Dark Matter and Cosmic Phenomena</t>
+          <t>Paleontology</t>
         </is>
       </c>
       <c r="B96">
@@ -1322,7 +1322,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Dentistry</t>
+          <t>Plant and animal studies</t>
         </is>
       </c>
       <c r="B97">
@@ -1332,7 +1332,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Earth-Surface Processes</t>
+          <t>Public Health, Environmental and Occupational Health</t>
         </is>
       </c>
       <c r="B98">
@@ -1342,7 +1342,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Endocrinology, Diabetes and Metabolism</t>
+          <t>Radiomics and Machine Learning in Medical Imaging</t>
         </is>
       </c>
       <c r="B99">
@@ -1352,7 +1352,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Environmental Engineering</t>
+          <t>Sociology and Political Science</t>
         </is>
       </c>
       <c r="B100">
@@ -1362,7 +1362,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Finance</t>
+          <t>Ultrasonics and Acoustic Wave Propagation</t>
         </is>
       </c>
       <c r="B101">
@@ -1372,7 +1372,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Hematology</t>
+          <t>Water Science and Technology</t>
         </is>
       </c>
       <c r="B102">
@@ -1382,167 +1382,167 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Hepatology</t>
+          <t>ATP Synthase and ATPases Research</t>
         </is>
       </c>
       <c r="B103">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Immunology and Microbiology</t>
+          <t>Accounting</t>
         </is>
       </c>
       <c r="B104">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Infectious Diseases and Tuberculosis</t>
+          <t>Advanced Fluorescence Microscopy Techniques</t>
         </is>
       </c>
       <c r="B105">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Liver Disease Diagnosis and Treatment</t>
+          <t>Advanced Memory and Neural Computing</t>
         </is>
       </c>
       <c r="B106">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Liver Disease and Transplantation</t>
+          <t>Advanced Surface Polishing Techniques</t>
         </is>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Neuroscience</t>
+          <t>Aging</t>
         </is>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Oral Health Pathology and Treatment</t>
+          <t>Agriculture and Farm Safety</t>
         </is>
       </c>
       <c r="B109">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Pancreatic and Hepatic Oncology Research</t>
+          <t>Applied Mathematics</t>
         </is>
       </c>
       <c r="B110">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Pathology and Forensic Medicine</t>
+          <t>Aquatic Science</t>
         </is>
       </c>
       <c r="B111">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Periodontics</t>
+          <t>Astrophysical Phenomena and Observations</t>
         </is>
       </c>
       <c r="B112">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Pollution</t>
+          <t>Biophysics</t>
         </is>
       </c>
       <c r="B113">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Public Health, Environmental and Occupational Health</t>
+          <t>Body Contouring and Surgery</t>
         </is>
       </c>
       <c r="B114">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Radio Astronomy Observations and Technology</t>
+          <t>Brain Tumor Detection and Classification</t>
         </is>
       </c>
       <c r="B115">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Remote Sensing in Agriculture</t>
+          <t>Business, Management and Accounting</t>
         </is>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Social Psychology</t>
+          <t>CCD and CMOS Imaging Sensors</t>
         </is>
       </c>
       <c r="B117">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Solar and Space Plasma Dynamics</t>
+          <t>COVID-19 Clinical Research Studies</t>
         </is>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>AI in cancer detection</t>
+          <t>COVID-19 and Mental Health</t>
         </is>
       </c>
       <c r="B119">
@@ -1552,7 +1552,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Advanced Measurement and Metrology Techniques</t>
+          <t>Cancer, Hypoxia, and Metabolism</t>
         </is>
       </c>
       <c r="B120">
@@ -1562,7 +1562,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Advanced Surface Polishing Techniques</t>
+          <t>Cell Biology</t>
         </is>
       </c>
       <c r="B121">
@@ -1572,7 +1572,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Air Quality and Health Impacts</t>
+          <t>Chemical Engineering</t>
         </is>
       </c>
       <c r="B122">
@@ -1582,7 +1582,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Appendicitis Diagnosis and Management</t>
+          <t>Chemical Thermodynamics and Molecular Structure</t>
         </is>
       </c>
       <c r="B123">
@@ -1592,7 +1592,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Astronomical Observations and Instrumentation</t>
+          <t>Community Health and Development</t>
         </is>
       </c>
       <c r="B124">
@@ -1602,7 +1602,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Bone fractures and treatments</t>
+          <t>Complex Systems and Time Series Analysis</t>
         </is>
       </c>
       <c r="B125">
@@ -1612,7 +1612,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Cervical Cancer and HPV Research</t>
+          <t>Control and Systems Engineering</t>
         </is>
       </c>
       <c r="B126">
@@ -1622,7 +1622,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Climate Change and Health Impacts</t>
+          <t>Cultural Differences and Values</t>
         </is>
       </c>
       <c r="B127">
@@ -1632,7 +1632,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Climate change and permafrost</t>
+          <t>Decision Sciences</t>
         </is>
       </c>
       <c r="B128">
@@ -1642,7 +1642,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Clinical Psychology</t>
+          <t>Diabetes Management and Education</t>
         </is>
       </c>
       <c r="B129">
@@ -1652,7 +1652,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Complementary and alternative medicine</t>
+          <t>Diet and metabolism studies</t>
         </is>
       </c>
       <c r="B130">
@@ -1662,7 +1662,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Corporate Finance and Governance</t>
+          <t>Ecological Modeling</t>
         </is>
       </c>
       <c r="B131">
@@ -1672,7 +1672,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Critical Care and Intensive Care Medicine</t>
+          <t>Ecology and Vegetation Dynamics Studies</t>
         </is>
       </c>
       <c r="B132">
@@ -1682,7 +1682,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Decision Sciences</t>
+          <t>Education</t>
         </is>
       </c>
       <c r="B133">
@@ -1692,7 +1692,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Demographic Trends and Gender Preferences</t>
+          <t>Emergency Medicine</t>
         </is>
       </c>
       <c r="B134">
@@ -1702,7 +1702,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Diabetes and associated disorders</t>
+          <t>Energy and Environment Impacts</t>
         </is>
       </c>
       <c r="B135">
@@ -1712,7 +1712,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Ecological Modeling</t>
+          <t>Epilepsy research and treatment</t>
         </is>
       </c>
       <c r="B136">
@@ -1722,7 +1722,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Ecology and Vegetation Dynamics Studies</t>
+          <t>Esophageal Cancer Research and Treatment</t>
         </is>
       </c>
       <c r="B137">
@@ -1732,7 +1732,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Ecology, Evolution, Behavior and Systematics</t>
+          <t>Financial Markets and Investment Strategies</t>
         </is>
       </c>
       <c r="B138">
@@ -1742,7 +1742,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Economics and Econometrics</t>
+          <t>Gastroesophageal reflux and treatments</t>
         </is>
       </c>
       <c r="B139">
@@ -1752,7 +1752,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Environmental Chemistry</t>
+          <t>Gastrointestinal motility and disorders</t>
         </is>
       </c>
       <c r="B140">
@@ -1762,7 +1762,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Financial Markets and Investment Strategies</t>
+          <t>Genetic and Clinical Aspects of Sex Determination and Chromosomal Abnormalities</t>
         </is>
       </c>
       <c r="B141">
@@ -1772,7 +1772,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>Fungal Infections and Studies</t>
+          <t>Genetics and Neurodevelopmental Disorders</t>
         </is>
       </c>
       <c r="B142">
@@ -1782,7 +1782,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Gastroenterology</t>
+          <t>Genetics, Aging, and Longevity in Model Organisms</t>
         </is>
       </c>
       <c r="B143">
@@ -1792,7 +1792,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Gender Studies</t>
+          <t>Genomics and Rare Diseases</t>
         </is>
       </c>
       <c r="B144">
@@ -1802,7 +1802,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Geography Education and Pedagogy</t>
+          <t>Hematology</t>
         </is>
       </c>
       <c r="B145">
@@ -1812,7 +1812,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Geography, Planning and Development</t>
+          <t>Human-Computer Interaction</t>
         </is>
       </c>
       <c r="B146">
@@ -1822,7 +1822,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Geological formations and processes</t>
+          <t>Hydrology and Watershed Management Studies</t>
         </is>
       </c>
       <c r="B147">
@@ -1832,7 +1832,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Global Cancer Incidence and Screening</t>
+          <t>Immunology</t>
         </is>
       </c>
       <c r="B148">
@@ -1842,7 +1842,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Heavy Metal Exposure and Toxicity</t>
+          <t>Inorganic Chemistry</t>
         </is>
       </c>
       <c r="B149">
@@ -1852,7 +1852,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Heavy metals in environment</t>
+          <t>Ionosphere and magnetosphere dynamics</t>
         </is>
       </c>
       <c r="B150">
@@ -1862,7 +1862,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Hematopoietic Stem Cell Transplantation</t>
+          <t>Isotope Analysis in Ecology</t>
         </is>
       </c>
       <c r="B151">
@@ -1872,7 +1872,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>High Altitude and Hypoxia</t>
+          <t>Laser Material Processing Techniques</t>
         </is>
       </c>
       <c r="B152">
@@ -1882,7 +1882,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Intensive Care Unit Cognitive Disorders</t>
+          <t>Liver Disease Diagnosis and Treatment</t>
         </is>
       </c>
       <c r="B153">
@@ -1892,7 +1892,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Ionosphere and magnetosphere dynamics</t>
+          <t>Long-Term Effects of COVID-19</t>
         </is>
       </c>
       <c r="B154">
@@ -1902,7 +1902,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Landslides and related hazards</t>
+          <t>Management Science and Operations Research</t>
         </is>
       </c>
       <c r="B155">
@@ -1912,7 +1912,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Long-Term Effects of COVID-19</t>
+          <t>Maternal Mental Health During Pregnancy and Postpartum</t>
         </is>
       </c>
       <c r="B156">
@@ -1922,7 +1922,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Lung Cancer Diagnosis and Treatment</t>
+          <t>Medical Imaging and Analysis</t>
         </is>
       </c>
       <c r="B157">
@@ -1932,7 +1932,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Management, Monitoring, Policy and Law</t>
+          <t>Mental Health Treatment and Access</t>
         </is>
       </c>
       <c r="B158">
@@ -1942,7 +1942,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Metal and Thin Film Mechanics</t>
         </is>
       </c>
       <c r="B159">
@@ -1952,7 +1952,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Media Technology</t>
+          <t>Ocean Engineering</t>
         </is>
       </c>
       <c r="B160">
@@ -1962,7 +1962,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Meteorological Phenomena and Simulations</t>
+          <t>Pediatrics, Perinatology and Child Health</t>
         </is>
       </c>
       <c r="B161">
@@ -1972,7 +1972,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Nature and Landscape Conservation</t>
+          <t>Pharmacology</t>
         </is>
       </c>
       <c r="B162">
@@ -1982,7 +1982,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Optical Polarization and Ellipsometry</t>
+          <t>Physical and Theoretical Chemistry</t>
         </is>
       </c>
       <c r="B163">
@@ -1992,7 +1992,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Pharmacology</t>
+          <t>Plant Molecular Biology Research</t>
         </is>
       </c>
       <c r="B164">
@@ -2002,7 +2002,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Planetary Science and Exploration</t>
+          <t>Polar Research and Ecology</t>
         </is>
       </c>
       <c r="B165">
@@ -2012,7 +2012,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Pneumonia and Respiratory Infections</t>
+          <t>Pollution</t>
         </is>
       </c>
       <c r="B166">
@@ -2022,7 +2022,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Psychiatry and Mental health</t>
+          <t>Primate Behavior and Ecology</t>
         </is>
       </c>
       <c r="B167">
@@ -2032,7 +2032,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Radiomics and Machine Learning in Medical Imaging</t>
+          <t>Protist diversity and phylogeny</t>
         </is>
       </c>
       <c r="B168">
@@ -2042,7 +2042,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Rehabilitation</t>
+          <t>Psychiatry and Mental health</t>
         </is>
       </c>
       <c r="B169">
@@ -2052,7 +2052,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Reproductive Medicine</t>
+          <t>Radio Astronomy Observations and Technology</t>
         </is>
       </c>
       <c r="B170">
@@ -2062,7 +2062,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>Respiratory Support and Mechanisms</t>
+          <t>Signal Processing</t>
         </is>
       </c>
       <c r="B171">
@@ -2072,7 +2072,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Respiratory viral infections research</t>
+          <t>Solar and Space Plasma Dynamics</t>
         </is>
       </c>
       <c r="B172">
@@ -2082,7 +2082,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>Sepsis Diagnosis and Treatment</t>
+          <t>Space Satellite Systems and Control</t>
         </is>
       </c>
       <c r="B173">
@@ -2112,7 +2112,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>Tree-ring climate responses</t>
+          <t>Spectroscopy and Laser Applications</t>
         </is>
       </c>
       <c r="B176">
@@ -2122,7 +2122,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Ultrasonics and Acoustic Wave Propagation</t>
+          <t>Trace Elements in Health</t>
         </is>
       </c>
       <c r="B177">
@@ -2132,7 +2132,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Water Science and Technology</t>
+          <t>Tracheal and airway disorders</t>
         </is>
       </c>
       <c r="B178">
@@ -2142,37 +2142,37 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>ATP Synthase and ATPases Research</t>
+          <t>Vaccine Coverage and Hesitancy</t>
         </is>
       </c>
       <c r="B179">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Acute Ischemic Stroke Management</t>
+          <t>Viral gastroenteritis research and epidemiology</t>
         </is>
       </c>
       <c r="B180">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>Acute Myocardial Infarction Research</t>
+          <t>Voice and Speech Disorders</t>
         </is>
       </c>
       <c r="B181">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Adipose Tissue and Metabolism</t>
+          <t>Advanced Algebra and Geometry</t>
         </is>
       </c>
       <c r="B182">
@@ -2182,7 +2182,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Adsorption and biosorption for pollutant removal</t>
+          <t>Advanced Breast Cancer Therapies</t>
         </is>
       </c>
       <c r="B183">
@@ -2192,7 +2192,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Advanced NMR Techniques and Applications</t>
+          <t>Advanced Drug Delivery Systems</t>
         </is>
       </c>
       <c r="B184">
@@ -2202,7 +2202,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Advanced Optical Imaging Technologies</t>
+          <t>Advanced Fiber Laser Technologies</t>
         </is>
       </c>
       <c r="B185">
@@ -2212,7 +2212,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Advanced Sensor and Energy Harvesting Materials</t>
+          <t>Advanced Graph Theory Research</t>
         </is>
       </c>
       <c r="B186">
@@ -2222,7 +2222,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>Advanced Vision and Imaging</t>
+          <t>Advanced Image and Video Retrieval Techniques</t>
         </is>
       </c>
       <c r="B187">
@@ -2232,7 +2232,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>African Sexualities and LGBTQ+ Issues</t>
+          <t>Advanced Operator Algebra Research</t>
         </is>
       </c>
       <c r="B188">
@@ -2242,7 +2242,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Agricultural pest management studies</t>
+          <t>Advanced Polymer Synthesis and Characterization</t>
         </is>
       </c>
       <c r="B189">
@@ -2252,7 +2252,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Air Quality Monitoring and Forecasting</t>
+          <t>Advanced Sensor and Energy Harvesting Materials</t>
         </is>
       </c>
       <c r="B190">
@@ -2262,7 +2262,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Airway Management and Intubation Techniques</t>
+          <t>Advanced Text Analysis Techniques</t>
         </is>
       </c>
       <c r="B191">
@@ -2272,7 +2272,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Alcohol Consumption and Health Effects</t>
+          <t>Advanced Topics in Algebra</t>
         </is>
       </c>
       <c r="B192">
@@ -2282,7 +2282,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Algebra and Number Theory</t>
+          <t>Advanced machining processes and optimization</t>
         </is>
       </c>
       <c r="B193">
@@ -2292,7 +2292,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Algebraic Geometry and Number Theory</t>
+          <t>Advanced optical system design</t>
         </is>
       </c>
       <c r="B194">
@@ -2302,7 +2302,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Algebraic and Geometric Analysis</t>
+          <t>Aerodynamics and Fluid Dynamics Research</t>
         </is>
       </c>
       <c r="B195">
@@ -2312,7 +2312,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Analytic Number Theory Research</t>
+          <t>Agriculture Sustainability and Environmental Impact</t>
         </is>
       </c>
       <c r="B196">
@@ -2322,7 +2322,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Anesthesiology and Pain Medicine</t>
+          <t>Agronomy and Crop Science</t>
         </is>
       </c>
       <c r="B197">
@@ -2332,7 +2332,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Angiogenesis and VEGF in Cancer</t>
+          <t>Airway Management and Intubation Techniques</t>
         </is>
       </c>
       <c r="B198">
@@ -2342,7 +2342,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Animal Vocal Communication and Behavior</t>
+          <t>Algebra and Number Theory</t>
         </is>
       </c>
       <c r="B199">
@@ -2352,7 +2352,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Animal and Plant Science Education</t>
+          <t>Algebraic and Geometric Analysis</t>
         </is>
       </c>
       <c r="B200">
@@ -2362,7 +2362,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Anthropology</t>
+          <t>Alzheimer's disease research and treatments</t>
         </is>
       </c>
       <c r="B201">
@@ -2372,7 +2372,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Antiplatelet Therapy and Cardiovascular Diseases</t>
+          <t>Amoebic Infections and Treatments</t>
         </is>
       </c>
       <c r="B202">
@@ -2382,7 +2382,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Applied Mathematics</t>
+          <t>Amphibian and Reptile Biology</t>
         </is>
       </c>
       <c r="B203">
@@ -2392,7 +2392,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Arsenic contamination and mitigation</t>
+          <t>Analytical Chemistry and Sensors</t>
         </is>
       </c>
       <c r="B204">
@@ -2402,7 +2402,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Artificial Intelligence in Healthcare and Education</t>
+          <t>Anesthesiology and Pain Medicine</t>
         </is>
       </c>
       <c r="B205">
@@ -2412,7 +2412,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Assisted Reproductive Technology and Twin Pregnancy</t>
+          <t>Animal Disease Management and Epidemiology</t>
         </is>
       </c>
       <c r="B206">
@@ -2422,7 +2422,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>Asthma and respiratory diseases</t>
+          <t>Animal Ecology and Behavior Studies</t>
         </is>
       </c>
       <c r="B207">
@@ -2432,7 +2432,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Atomic and Subatomic Physics Research</t>
+          <t>Antimicrobial Peptides and Activities</t>
         </is>
       </c>
       <c r="B208">
@@ -2442,7 +2442,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Attention Deficit Hyperactivity Disorder</t>
+          <t>Aquaculture disease management and microbiota</t>
         </is>
       </c>
       <c r="B209">
@@ -2452,7 +2452,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Auction Theory and Applications</t>
+          <t>Architecture</t>
         </is>
       </c>
       <c r="B210">
@@ -2462,7 +2462,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Auditing, Earnings Management, Governance</t>
+          <t>Asymmetric Hydrogenation and Catalysis</t>
         </is>
       </c>
       <c r="B211">
@@ -2472,7 +2472,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Autism Spectrum Disorder Research</t>
+          <t>Atmospheric Ozone and Climate</t>
         </is>
       </c>
       <c r="B212">
@@ -2482,7 +2482,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Bioactive Compounds and Antitumor Agents</t>
+          <t>Atmospheric aerosols and clouds</t>
         </is>
       </c>
       <c r="B213">
@@ -2492,7 +2492,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Biomaterials</t>
+          <t>Atmospheric and Environmental Gas Dynamics</t>
         </is>
       </c>
       <c r="B214">
@@ -2502,7 +2502,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Biosensors and Analytical Detection</t>
+          <t>Atmospheric chemistry and aerosols</t>
         </is>
       </c>
       <c r="B215">
@@ -2512,7 +2512,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Black Holes and Theoretical Physics</t>
+          <t>Auditing, Earnings Management, Governance</t>
         </is>
       </c>
       <c r="B216">
@@ -2522,7 +2522,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>CCD and CMOS Imaging Sensors</t>
+          <t>Banana Cultivation and Research</t>
         </is>
       </c>
       <c r="B217">
@@ -2532,7 +2532,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>COVID-19 Pandemic Impacts</t>
+          <t>Bat Biology and Ecology Studies</t>
         </is>
       </c>
       <c r="B218">
@@ -2542,7 +2542,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>COVID-19 and Mental Health</t>
+          <t>Biochemical Analysis and Sensing Techniques</t>
         </is>
       </c>
       <c r="B219">
@@ -2552,7 +2552,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>Calibration and Measurement Techniques</t>
+          <t>Biochemical and Molecular Research</t>
         </is>
       </c>
       <c r="B220">
@@ -2562,7 +2562,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>Cancer Immunotherapy and Biomarkers</t>
+          <t>Bioengineering</t>
         </is>
       </c>
       <c r="B221">
@@ -2572,7 +2572,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>Cancer Research</t>
+          <t>Bioinformatics and Genomic Networks</t>
         </is>
       </c>
       <c r="B222">
@@ -2582,7 +2582,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>Cancer Treatment and Pharmacology</t>
+          <t>Biomaterials</t>
         </is>
       </c>
       <c r="B223">
@@ -2592,7 +2592,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>Cancer survivorship and care</t>
+          <t>Biomedical and Engineering Education</t>
         </is>
       </c>
       <c r="B224">
@@ -2602,7 +2602,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>Cancer therapeutics and mechanisms</t>
+          <t>Bladder and Urothelial Cancer Treatments</t>
         </is>
       </c>
       <c r="B225">
@@ -2612,7 +2612,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>Cancer, Hypoxia, and Metabolism</t>
+          <t>Blockchain Technology Applications and Security</t>
         </is>
       </c>
       <c r="B226">
@@ -2622,7 +2622,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>Cannabis and Cannabinoid Research</t>
+          <t>Blood Coagulation and Thrombosis Mechanisms</t>
         </is>
       </c>
       <c r="B227">
@@ -2632,7 +2632,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>Carbon Dioxide Capture Technologies</t>
+          <t>Blood properties and coagulation</t>
         </is>
       </c>
       <c r="B228">
@@ -2642,7 +2642,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>Cardiac Arrest and Resuscitation</t>
+          <t>Breast Cancer Treatment Studies</t>
         </is>
       </c>
       <c r="B229">
@@ -2652,7 +2652,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Cardiac Arrhythmias and Treatments</t>
+          <t>COVID-19 Pandemic Impacts</t>
         </is>
       </c>
       <c r="B230">
@@ -2662,7 +2662,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Cardiac electrophysiology and arrhythmias</t>
+          <t>COVID-19 epidemiological studies</t>
         </is>
       </c>
       <c r="B231">
@@ -2672,7 +2672,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Cardiac pacing and defibrillation studies</t>
+          <t>Calibration and Measurement Techniques</t>
         </is>
       </c>
       <c r="B232">
@@ -2682,7 +2682,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Cardiovascular Disease and Adiposity</t>
+          <t>Cardiac Arrest and Resuscitation</t>
         </is>
       </c>
       <c r="B233">
@@ -2692,7 +2692,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Catalysis</t>
+          <t>Cardiac Arrhythmias and Treatments</t>
         </is>
       </c>
       <c r="B234">
@@ -2702,7 +2702,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Cellular and Molecular Neuroscience</t>
+          <t>Cardiac Health and Mental Health</t>
         </is>
       </c>
       <c r="B235">
@@ -2712,7 +2712,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Cellular transport and secretion</t>
+          <t>Cardiac Structural Anomalies and Repair</t>
         </is>
       </c>
       <c r="B236">
@@ -2722,7 +2722,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Chaos control and synchronization</t>
+          <t>Cardiac electrophysiology and arrhythmias</t>
         </is>
       </c>
       <c r="B237">
@@ -2732,7 +2732,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Chemical Engineering</t>
+          <t>Cardiac pacing and defibrillation studies</t>
         </is>
       </c>
       <c r="B238">
@@ -2742,7 +2742,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Chemistry and Chemical Engineering</t>
+          <t>Cardiovascular Disease and Adiposity</t>
         </is>
       </c>
       <c r="B239">
@@ -2752,7 +2752,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Child and Adolescent Health</t>
+          <t>Cardiovascular Health and Risk Factors</t>
         </is>
       </c>
       <c r="B240">
@@ -2762,7 +2762,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Cholangiocarcinoma and Gallbladder Cancer Studies</t>
+          <t>Catalysis</t>
         </is>
       </c>
       <c r="B241">
@@ -2772,7 +2772,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Climate Change Communication and Perception</t>
+          <t>Catalysts for Methane Reforming</t>
         </is>
       </c>
       <c r="B242">
@@ -2782,7 +2782,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>Climate Change and Geoengineering</t>
+          <t>Catalytic C–H Functionalization Methods</t>
         </is>
       </c>
       <c r="B243">
@@ -2792,7 +2792,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>Climate change impacts on agriculture</t>
+          <t>Cell death mechanisms and regulation</t>
         </is>
       </c>
       <c r="B244">
@@ -2802,7 +2802,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>Coal and Its By-products</t>
+          <t>Cellular and Molecular Neuroscience</t>
         </is>
       </c>
       <c r="B245">
@@ -2812,7 +2812,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>Coding theory and cryptography</t>
+          <t>Cervical Cancer and HPV Research</t>
         </is>
       </c>
       <c r="B246">
@@ -2822,7 +2822,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>Cognitive Neuroscience</t>
+          <t>Child Nutrition and Water Access</t>
         </is>
       </c>
       <c r="B247">
@@ -2832,7 +2832,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>Cold Atom Physics and Bose-Einstein Condensates</t>
+          <t>Child and Adolescent Psychosocial and Emotional Development</t>
         </is>
       </c>
       <c r="B248">
@@ -2842,7 +2842,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>Complementary and Alternative Medicine Studies</t>
+          <t>Chronic Disease Management Strategies</t>
         </is>
       </c>
       <c r="B249">
@@ -2852,7 +2852,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>Complex Systems and Time Series Analysis</t>
+          <t>Climate Change Communication and Perception</t>
         </is>
       </c>
       <c r="B250">
@@ -2862,7 +2862,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>Computational Drug Discovery Methods</t>
+          <t>Climate Change and Geoengineering</t>
         </is>
       </c>
       <c r="B251">
@@ -2872,7 +2872,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>Computer Networks and Communications</t>
+          <t>Climate Change and Health Impacts</t>
         </is>
       </c>
       <c r="B252">
@@ -2882,7 +2882,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>Computer Science Applications</t>
+          <t>Climate change impacts on agriculture</t>
         </is>
       </c>
       <c r="B253">
@@ -2892,7 +2892,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>Concrete Corrosion and Durability</t>
+          <t>Clinical Biochemistry</t>
         </is>
       </c>
       <c r="B254">
@@ -2902,7 +2902,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>Consumer Market Behavior and Pricing</t>
+          <t>Cloud Computing and Resource Management</t>
         </is>
       </c>
       <c r="B255">
@@ -2912,7 +2912,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>Contact Mechanics and Variational Inequalities</t>
+          <t>Complementary and alternative medicine</t>
         </is>
       </c>
       <c r="B256">
@@ -2922,7 +2922,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>Corneal surgery and disorders</t>
+          <t>Computational Drug Discovery Methods</t>
         </is>
       </c>
       <c r="B257">
@@ -2932,7 +2932,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>Cultural Studies</t>
+          <t>Computational Fluid Dynamics and Aerodynamics</t>
         </is>
       </c>
       <c r="B258">
@@ -2942,7 +2942,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>Customer Service Quality and Loyalty</t>
+          <t>Concrete and Cement Materials Research</t>
         </is>
       </c>
       <c r="B259">
@@ -2952,7 +2952,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>Dam Engineering and Safety</t>
+          <t>Connective tissue disorders research</t>
         </is>
       </c>
       <c r="B260">
@@ -2962,7 +2962,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>Developmental Biology</t>
+          <t>Corporate Finance and Governance</t>
         </is>
       </c>
       <c r="B261">
@@ -2972,7 +2972,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>Diabetes Management and Research</t>
+          <t>Crystal structures of chemical compounds</t>
         </is>
       </c>
       <c r="B262">
@@ -2982,7 +2982,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>Diabetes Treatment and Management</t>
+          <t>Crystallography and molecular interactions</t>
         </is>
       </c>
       <c r="B263">
@@ -2992,7 +2992,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>Diabetes, Cardiovascular Risks, and Lipoproteins</t>
+          <t>Cutaneous Melanoma Detection and Management</t>
         </is>
       </c>
       <c r="B264">
@@ -3002,7 +3002,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>Diagnosis and treatment of tuberculosis</t>
+          <t>Dark Matter and Cosmic Phenomena</t>
         </is>
       </c>
       <c r="B265">
@@ -3012,7 +3012,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>Digital Holography and Microscopy</t>
+          <t>Dermatology</t>
         </is>
       </c>
       <c r="B266">
@@ -3022,7 +3022,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>Digital Media Forensic Detection</t>
+          <t>Diabetes, Cardiovascular Risks, and Lipoproteins</t>
         </is>
       </c>
       <c r="B267">
@@ -3032,7 +3032,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>Digital Platforms and Economics</t>
+          <t>Diamond and Carbon-based Materials Research</t>
         </is>
       </c>
       <c r="B268">
@@ -3042,7 +3042,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>Digital Storytelling and Education</t>
+          <t>Digital Imaging for Blood Diseases</t>
         </is>
       </c>
       <c r="B269">
@@ -3052,7 +3052,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>Ecosystem dynamics and resilience</t>
+          <t>Digital Radiography and Breast Imaging</t>
         </is>
       </c>
       <c r="B270">
@@ -3062,7 +3062,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>Education</t>
+          <t>Distributed and Parallel Computing Systems</t>
         </is>
       </c>
       <c r="B271">
@@ -3072,7 +3072,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>Elbow and Forearm Trauma Treatment</t>
+          <t>Drilling and Well Engineering</t>
         </is>
       </c>
       <c r="B272">
@@ -3082,7 +3082,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>Electrospun Nanofibers in Biomedical Applications</t>
+          <t>ECG Monitoring and Analysis</t>
         </is>
       </c>
       <c r="B273">
@@ -3092,7 +3092,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>Emergency Medical Services</t>
+          <t>Echinoderm biology and ecology</t>
         </is>
       </c>
       <c r="B274">
@@ -3102,7 +3102,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>Employment and Welfare Studies</t>
+          <t>Electrocatalysts for Energy Conversion</t>
         </is>
       </c>
       <c r="B275">
@@ -3112,7 +3112,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>Endometriosis Research and Treatment</t>
+          <t>Electromagnetic Simulation and Numerical Methods</t>
         </is>
       </c>
       <c r="B276">
@@ -3122,7 +3122,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>Energy</t>
+          <t>Employment and Welfare Studies</t>
         </is>
       </c>
       <c r="B277">
@@ -3132,7 +3132,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>Energy and Environment Impacts</t>
+          <t>Endocrinology</t>
         </is>
       </c>
       <c r="B278">
@@ -3142,7 +3142,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>Environmental remediation with nanomaterials</t>
+          <t>Endoplasmic Reticulum Stress and Disease</t>
         </is>
       </c>
       <c r="B279">
@@ -3152,7 +3152,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>Eosinophilic Esophagitis</t>
+          <t>Energy</t>
         </is>
       </c>
       <c r="B280">
@@ -3162,7 +3162,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>Error Correcting Code Techniques</t>
+          <t>Energy Efficient Wireless Sensor Networks</t>
         </is>
       </c>
       <c r="B281">
@@ -3172,7 +3172,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>Ethics in Clinical Research</t>
+          <t>Energy Harvesting in Wireless Networks</t>
         </is>
       </c>
       <c r="B282">
@@ -3182,7 +3182,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>Experimental and Cognitive Psychology</t>
+          <t>Engineering Education and Curriculum Development</t>
         </is>
       </c>
       <c r="B283">
@@ -3192,7 +3192,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>Face recognition and analysis</t>
+          <t>Engineering Education and Pedagogy</t>
         </is>
       </c>
       <c r="B284">
@@ -3202,7 +3202,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>Fatigue and fracture mechanics</t>
+          <t>Entomopathogenic Microorganisms in Pest Control</t>
         </is>
       </c>
       <c r="B285">
@@ -3212,7 +3212,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>Fecal contamination and water quality</t>
+          <t>Environmental DNA in Biodiversity Studies</t>
         </is>
       </c>
       <c r="B286">
@@ -3222,7 +3222,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>Focus Groups and Qualitative Methods</t>
+          <t>Eosinophilic Esophagitis</t>
         </is>
       </c>
       <c r="B287">
@@ -3232,7 +3232,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>Gastroesophageal reflux and treatments</t>
+          <t>Epigenetics and DNA Methylation</t>
         </is>
       </c>
       <c r="B288">
@@ -3242,7 +3242,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>Gastrointestinal Bleeding Diagnosis and Treatment</t>
+          <t>Esophageal and GI Pathology</t>
         </is>
       </c>
       <c r="B289">
@@ -3252,7 +3252,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>Gaussian Processes and Bayesian Inference</t>
+          <t>Evaluation and Performance Assessment</t>
         </is>
       </c>
       <c r="B290">
@@ -3262,7 +3262,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>Generative Adversarial Networks and Image Synthesis</t>
+          <t>Evolution and Paleontology Studies</t>
         </is>
       </c>
       <c r="B291">
@@ -3272,7 +3272,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>Genetic Neurodegenerative Diseases</t>
+          <t>Experimental and Cognitive Psychology</t>
         </is>
       </c>
       <c r="B292">
@@ -3282,7 +3282,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>Genetic and Environmental Crop Studies</t>
+          <t>Ferroelectric and Negative Capacitance Devices</t>
         </is>
       </c>
       <c r="B293">
@@ -3292,7 +3292,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>Genetics and Neurodevelopmental Disorders</t>
+          <t>Financial Risk and Volatility Modeling</t>
         </is>
       </c>
       <c r="B294">
@@ -3302,7 +3302,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>Genomics and Rare Diseases</t>
+          <t>Food Science</t>
         </is>
       </c>
       <c r="B295">
@@ -3312,7 +3312,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>Genomics, phytochemicals, and oxidative stress</t>
+          <t>Gait Recognition and Analysis</t>
         </is>
       </c>
       <c r="B296">
@@ -3322,7 +3322,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>Geochemistry and Petrology</t>
+          <t>Gas Dynamics and Kinetic Theory</t>
         </is>
       </c>
       <c r="B297">
@@ -3332,7 +3332,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>Geometry and Topology</t>
+          <t>Gastric Cancer Management and Outcomes</t>
         </is>
       </c>
       <c r="B298">
@@ -3342,7 +3342,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>Geophysics</t>
+          <t>Gaussian Processes and Bayesian Inference</t>
         </is>
       </c>
       <c r="B299">
@@ -3352,7 +3352,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>Geotechnical Engineering and Analysis</t>
+          <t>Gaze Tracking and Assistive Technology</t>
         </is>
       </c>
       <c r="B300">
@@ -3362,7 +3362,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>Geotechnical Engineering and Soil Mechanics</t>
+          <t>Gene Regulatory Network Analysis</t>
         </is>
       </c>
       <c r="B301">
@@ -3372,7 +3372,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>Glaucoma and retinal disorders</t>
+          <t>Genetics, Bioinformatics, and Biomedical Research</t>
         </is>
       </c>
       <c r="B302">
@@ -3382,7 +3382,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>Global Energy and Sustainability Research</t>
+          <t>Genomics and Phylogenetic Studies</t>
         </is>
       </c>
       <c r="B303">
@@ -3392,7 +3392,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>Greenhouse Technology and Climate Control</t>
+          <t>Geochemistry and Petrology</t>
         </is>
       </c>
       <c r="B304">
@@ -3402,7 +3402,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>Health Informatics</t>
+          <t>Geological and Geochemical Analysis</t>
         </is>
       </c>
       <c r="B305">
@@ -3412,7 +3412,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>Health, psychology, and well-being</t>
+          <t>Geomagnetism and Paleomagnetism Studies</t>
         </is>
       </c>
       <c r="B306">
@@ -3422,7 +3422,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>Healthcare Systems and Public Health</t>
+          <t>Geophysical Methods and Applications</t>
         </is>
       </c>
       <c r="B307">
@@ -3432,7 +3432,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>Healthcare Systems and Reforms</t>
+          <t>Geophysics</t>
         </is>
       </c>
       <c r="B308">
@@ -3442,7 +3442,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>Hematological disorders and diagnostics</t>
+          <t>Geophysics and Gravity Measurements</t>
         </is>
       </c>
       <c r="B309">
@@ -3452,7 +3452,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>Hippo pathway signaling and YAP/TAZ</t>
+          <t>Geotechnical Engineering and Underground Structures</t>
         </is>
       </c>
       <c r="B310">
@@ -3462,7 +3462,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>Homelessness and Social Issues</t>
+          <t>Global Maternal and Child Health</t>
         </is>
       </c>
       <c r="B311">
@@ -3472,7 +3472,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>Hydrogen's biological and therapeutic effects</t>
+          <t>Graph Labeling and Dimension Problems</t>
         </is>
       </c>
       <c r="B312">
@@ -3482,7 +3482,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>Hydrological Forecasting Using AI</t>
+          <t>Groundwater and Isotope Geochemistry</t>
         </is>
       </c>
       <c r="B313">
@@ -3492,7 +3492,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>Immunology</t>
+          <t>HER2/EGFR in Cancer Research</t>
         </is>
       </c>
       <c r="B314">
@@ -3502,7 +3502,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>Impact of Technology on Adolescents</t>
+          <t>HIV Research and Treatment</t>
         </is>
       </c>
       <c r="B315">
@@ -3512,7 +3512,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>Industrial and Manufacturing Engineering</t>
+          <t>HIV/AIDS Research and Interventions</t>
         </is>
       </c>
       <c r="B316">
@@ -3522,7 +3522,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>Infant Health and Development</t>
+          <t>HIV/AIDS oral health manifestations</t>
         </is>
       </c>
       <c r="B317">
@@ -3532,7 +3532,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>Inflammatory Bowel Disease</t>
+          <t>Hand Gesture Recognition Systems</t>
         </is>
       </c>
       <c r="B318">
@@ -3542,7 +3542,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>Influenza Virus Research Studies</t>
+          <t>Health Systems, Economic Evaluations, Quality of Life</t>
         </is>
       </c>
       <c r="B319">
@@ -3552,7 +3552,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>Information Systems</t>
+          <t>Health and Wellbeing Research</t>
         </is>
       </c>
       <c r="B320">
@@ -3562,7 +3562,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>Information Systems and Management</t>
+          <t>Health disparities and outcomes</t>
         </is>
       </c>
       <c r="B321">
@@ -3572,7 +3572,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>Internal Medicine</t>
+          <t>Heavy Metal Exposure and Toxicity</t>
         </is>
       </c>
       <c r="B322">
@@ -3582,7 +3582,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>Intestinal and Peritoneal Adhesions</t>
+          <t>Helicobacter pylori-related gastroenterology studies</t>
         </is>
       </c>
       <c r="B323">
@@ -3592,7 +3592,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>Ion Channels and Receptors</t>
+          <t>Hemoglobinopathies and Related Disorders</t>
         </is>
       </c>
       <c r="B324">
@@ -3602,7 +3602,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>Ionic liquids properties and applications</t>
+          <t>Hepatitis B Virus Studies</t>
         </is>
       </c>
       <c r="B325">
@@ -3612,7 +3612,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>Karst Systems and Hydrogeology</t>
+          <t>Hepatology</t>
         </is>
       </c>
       <c r="B326">
@@ -3622,7 +3622,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>LGBTQ Health, Identity, and Policy</t>
+          <t>High-Energy Particle Collisions Research</t>
         </is>
       </c>
       <c r="B327">
@@ -3632,7 +3632,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>Language and cultural evolution</t>
+          <t>Hip and Femur Fractures</t>
         </is>
       </c>
       <c r="B328">
@@ -3642,7 +3642,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>Laser Design and Applications</t>
+          <t>Human Pose and Action Recognition</t>
         </is>
       </c>
       <c r="B329">
@@ -3652,7 +3652,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>Laser Material Processing Techniques</t>
+          <t>Human-Animal Interaction Studies</t>
         </is>
       </c>
       <c r="B330">
@@ -3662,7 +3662,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>Legume Nitrogen Fixing Symbiosis</t>
+          <t>Hydrogels: synthesis, properties, applications</t>
         </is>
       </c>
       <c r="B331">
@@ -3672,7 +3672,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>Lipid metabolism and disorders</t>
+          <t>Hydrogen embrittlement and corrosion behaviors in metals</t>
         </is>
       </c>
       <c r="B332">
@@ -3682,7 +3682,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>Lipoproteins and Cardiovascular Health</t>
+          <t>Ichthyology and Marine Biology</t>
         </is>
       </c>
       <c r="B333">
@@ -3692,7 +3692,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>Lung Cancer Treatments and Mutations</t>
+          <t>Image Retrieval and Classification Techniques</t>
         </is>
       </c>
       <c r="B334">
@@ -3702,7 +3702,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>Magnesium in Health and Disease</t>
+          <t>Immunotherapy and Immune Responses</t>
         </is>
       </c>
       <c r="B335">
@@ -3712,7 +3712,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>Management Science and Operations Research</t>
+          <t>Industrial and Manufacturing Engineering</t>
         </is>
       </c>
       <c r="B336">
@@ -3722,7 +3722,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>Management of metastatic bone disease</t>
+          <t>Inertial Sensor and Navigation</t>
         </is>
       </c>
       <c r="B337">
@@ -3732,7 +3732,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>Mathematical Physics</t>
+          <t>Inflammatory mediators and NSAID effects</t>
         </is>
       </c>
       <c r="B338">
@@ -3742,7 +3742,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>Mathematics Education and Programs</t>
+          <t>Influenza Virus Research Studies</t>
         </is>
       </c>
       <c r="B339">
@@ -3752,7 +3752,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>Matrix Theory and Algorithms</t>
+          <t>Information Retrieval and Search Behavior</t>
         </is>
       </c>
       <c r="B340">
@@ -3762,7 +3762,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>Medical and Biological Ozone Research</t>
+          <t>Innovative Teaching Methods</t>
         </is>
       </c>
       <c r="B341">
@@ -3772,7 +3772,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>Medicinal Plant Extracts Effects</t>
+          <t>Insect Resistance and Genetics</t>
         </is>
       </c>
       <c r="B342">
@@ -3782,7 +3782,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>Melanoma and MAPK Pathways</t>
+          <t>Insect Science</t>
         </is>
       </c>
       <c r="B343">
@@ -3792,7 +3792,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>Mental Health Treatment and Access</t>
+          <t>Internal Medicine</t>
         </is>
       </c>
       <c r="B344">
@@ -3802,7 +3802,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>Mental Health and Patient Involvement</t>
+          <t>Internet Traffic Analysis and Secure E-voting</t>
         </is>
       </c>
       <c r="B345">
@@ -3812,7 +3812,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>Misinformation and Its Impacts</t>
+          <t>IoT and Edge/Fog Computing</t>
         </is>
       </c>
       <c r="B346">
@@ -3822,7 +3822,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>Mitochondrial Function and Pathology</t>
+          <t>Ion-surface interactions and analysis</t>
         </is>
       </c>
       <c r="B347">
@@ -3832,7 +3832,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>Mobile Learning in Education</t>
+          <t>Iron Metabolism and Disorders</t>
         </is>
       </c>
       <c r="B348">
@@ -3842,7 +3842,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>Model Reduction and Neural Networks</t>
+          <t>Laser-Matter Interactions and Applications</t>
         </is>
       </c>
       <c r="B349">
@@ -3852,7 +3852,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>Modeling and Simulation</t>
+          <t>Lipoproteins and Cardiovascular Health</t>
         </is>
       </c>
       <c r="B350">
@@ -3862,7 +3862,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>Molecular Junctions and Nanostructures</t>
+          <t>Liver Disease and Transplantation</t>
         </is>
       </c>
       <c r="B351">
@@ -3872,7 +3872,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>Multiple Myeloma Research and Treatments</t>
+          <t>Machine Learning in Bioinformatics</t>
         </is>
       </c>
       <c r="B352">
@@ -3882,7 +3882,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>Musculoskeletal Disorders and Rehabilitation</t>
+          <t>Machine Learning in Healthcare</t>
         </is>
       </c>
       <c r="B353">
@@ -3892,7 +3892,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>Mycobacterium research and diagnosis</t>
+          <t>Marine Biology and Ecology Research</t>
         </is>
       </c>
       <c r="B354">
@@ -3902,7 +3902,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>Nail Diseases and Treatments</t>
+          <t>Materials Chemistry</t>
         </is>
       </c>
       <c r="B355">
@@ -3912,7 +3912,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>Nanoplatforms for cancer theranostics</t>
+          <t>Mechanical Circulatory Support Devices</t>
         </is>
       </c>
       <c r="B356">
@@ -3922,7 +3922,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>Neuroblastoma Research and Treatments</t>
+          <t>Media Technology</t>
         </is>
       </c>
       <c r="B357">
@@ -3932,7 +3932,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>Neuroendocrine Tumor Research Advances</t>
+          <t>Medical and Biological Ozone Research</t>
         </is>
       </c>
       <c r="B358">
@@ -3942,7 +3942,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>Noncommutative and Quantum Gravity Theories</t>
+          <t>Menopause: Health Impacts and Treatments</t>
         </is>
       </c>
       <c r="B359">
@@ -3952,7 +3952,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>Nuclear Structure and Function</t>
+          <t>Metabolism and Genetic Disorders</t>
         </is>
       </c>
       <c r="B360">
@@ -3962,7 +3962,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>Numerical Analysis</t>
+          <t>Metaheuristic Optimization Algorithms Research</t>
         </is>
       </c>
       <c r="B361">
@@ -3972,7 +3972,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>Numerical methods for differential equations</t>
+          <t>Metals and Alloys</t>
         </is>
       </c>
       <c r="B362">
@@ -3982,7 +3982,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>Nutrition and Health in Aging</t>
+          <t>Meteorological Phenomena and Simulations</t>
         </is>
       </c>
       <c r="B363">
@@ -3992,7 +3992,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>Nutrition, Genetics, and Disease</t>
+          <t>Microbial Community Ecology and Physiology</t>
         </is>
       </c>
       <c r="B364">
@@ -4002,7 +4002,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>Oceanographic and Atmospheric Processes</t>
+          <t>Microbiology</t>
         </is>
       </c>
       <c r="B365">
@@ -4012,7 +4012,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>Oceanography</t>
+          <t>Microgrid Control and Optimization</t>
         </is>
       </c>
       <c r="B366">
@@ -4022,7 +4022,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>Online Learning and Analytics</t>
+          <t>Microstructure and Mechanical Properties of Steels</t>
         </is>
       </c>
       <c r="B367">
@@ -4032,7 +4032,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>Ophthalmology</t>
+          <t>Mobile Ad Hoc Networks</t>
         </is>
       </c>
       <c r="B368">
@@ -4042,7 +4042,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>Ophthalmology and Visual Impairment Studies</t>
+          <t>Model Reduction and Neural Networks</t>
         </is>
       </c>
       <c r="B369">
@@ -4052,7 +4052,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>Optical Coatings and Gratings</t>
+          <t>Modeling and Simulation</t>
         </is>
       </c>
       <c r="B370">
@@ -4062,7 +4062,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>Optical measurement and interference techniques</t>
+          <t>Molecular Medicine</t>
         </is>
       </c>
       <c r="B371">
@@ -4072,7 +4072,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>Organic Chemistry Cycloaddition Reactions</t>
+          <t>Muscle metabolism and nutrition</t>
         </is>
       </c>
       <c r="B372">
@@ -4082,7 +4082,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>Organic Electronics and Photovoltaics</t>
+          <t>Music Therapy and Health</t>
         </is>
       </c>
       <c r="B373">
@@ -4092,7 +4092,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>Organic Light-Emitting Diodes Research</t>
+          <t>Music and Audio Processing</t>
         </is>
       </c>
       <c r="B374">
@@ -4102,7 +4102,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>Organizational Behavior and Human Resource Management</t>
+          <t>Myasthenia Gravis and Thymoma</t>
         </is>
       </c>
       <c r="B375">
@@ -4112,7 +4112,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>Orthopedic Surgery and Rehabilitation</t>
+          <t>Nasal Surgery and Airway Studies</t>
         </is>
       </c>
       <c r="B376">
@@ -4122,7 +4122,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>Osteomyelitis and Bone Disorders Research</t>
+          <t>Nematode management and characterization studies</t>
         </is>
       </c>
       <c r="B377">
@@ -4132,7 +4132,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>Parasitic Infections and Diagnostics</t>
+          <t>Network Security and Intrusion Detection</t>
         </is>
       </c>
       <c r="B378">
@@ -4142,7 +4142,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>Parasitology</t>
+          <t>Neuroendocrine regulation and behavior</t>
         </is>
       </c>
       <c r="B379">
@@ -4152,7 +4152,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>Parkinson's Disease Mechanisms and Treatments</t>
+          <t>Neurological disorders and treatments</t>
         </is>
       </c>
       <c r="B380">
@@ -4162,7 +4162,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>Particle Detector Development and Performance</t>
+          <t>Nonmelanoma Skin Cancer Studies</t>
         </is>
       </c>
       <c r="B381">
@@ -4172,7 +4172,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>Pediatric health and respiratory diseases</t>
+          <t>Numerical methods in engineering</t>
         </is>
       </c>
       <c r="B382">
@@ -4182,7 +4182,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>Peripheral Artery Disease Management</t>
+          <t>Obesity and Health Practices</t>
         </is>
       </c>
       <c r="B383">
@@ -4192,7 +4192,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>Pharmacology, Toxicology and Pharmaceutics</t>
+          <t>Obstructive Sleep Apnea Research</t>
         </is>
       </c>
       <c r="B384">
@@ -4202,7 +4202,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>Pharmacy</t>
+          <t>Oceanographic and Atmospheric Processes</t>
         </is>
       </c>
       <c r="B385">
@@ -4212,7 +4212,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>Phase Equilibria and Thermodynamics</t>
+          <t>Optical Coherence Tomography Applications</t>
         </is>
       </c>
       <c r="B386">
@@ -4222,7 +4222,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>Photodynamic Therapy Research Studies</t>
+          <t>Optical Network Technologies</t>
         </is>
       </c>
       <c r="B387">
@@ -4232,7 +4232,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>Photorefractive and Nonlinear Optics</t>
+          <t>Optimal Power Flow Distribution</t>
         </is>
       </c>
       <c r="B388">
@@ -4242,7 +4242,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>Plant Gene Expression Analysis</t>
+          <t>Organic Food and Agriculture</t>
         </is>
       </c>
       <c r="B389">
@@ -4252,7 +4252,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>Plant Molecular Biology Research</t>
+          <t>PARP inhibition in cancer therapy</t>
         </is>
       </c>
       <c r="B390">
@@ -4262,7 +4262,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>Plant Reproductive Biology</t>
+          <t>Paleontology and Evolutionary Biology</t>
         </is>
       </c>
       <c r="B391">
@@ -4272,7 +4272,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>Plant Stress Responses and Tolerance</t>
+          <t>Paleontology and Stratigraphy of Fossils</t>
         </is>
       </c>
       <c r="B392">
@@ -4282,7 +4282,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>Plant Water Relations and Carbon Dynamics</t>
+          <t>Pancreatic and Hepatic Oncology Research</t>
         </is>
       </c>
       <c r="B393">
@@ -4292,7 +4292,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>Plant and animal studies</t>
+          <t>Pancreatitis Pathology and Treatment</t>
         </is>
       </c>
       <c r="B394">
@@ -4302,7 +4302,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>Pleistocene-Era Hominins and Archaeology</t>
+          <t>Parkinson's Disease Mechanisms and Treatments</t>
         </is>
       </c>
       <c r="B395">
@@ -4312,7 +4312,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>Pneumocystis jirovecii pneumonia detection and treatment</t>
+          <t>Participatory Visual Research Methods</t>
         </is>
       </c>
       <c r="B396">
@@ -4322,7 +4322,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>Polydiacetylene-based materials and applications</t>
+          <t>Particle physics theoretical and experimental studies</t>
         </is>
       </c>
       <c r="B397">
@@ -4332,7 +4332,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>Precipitation Measurement and Analysis</t>
+          <t>Pediatric Urology and Nephrology Studies</t>
         </is>
       </c>
       <c r="B398">
@@ -4342,7 +4342,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>Pregnancy and preeclampsia studies</t>
+          <t>Pharmaceutical Science</t>
         </is>
       </c>
       <c r="B399">
@@ -4352,7 +4352,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>Preterm Birth and Chorioamnionitis</t>
+          <t>Pharmacology, Toxicology and Pharmaceutics</t>
         </is>
       </c>
       <c r="B400">
@@ -4362,7 +4362,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>Protein Degradation and Inhibitors</t>
+          <t>Pharmacy</t>
         </is>
       </c>
       <c r="B401">
@@ -4372,7 +4372,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>Protein Kinase Regulation and GTPase Signaling</t>
+          <t>Photoacoustic and Ultrasonic Imaging</t>
         </is>
       </c>
       <c r="B402">
@@ -4382,7 +4382,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>Protein Tyrosine Phosphatases</t>
+          <t>Photochemistry and Electron Transfer Studies</t>
         </is>
       </c>
       <c r="B403">
@@ -4392,7 +4392,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>Pulsars and Gravitational Waves Research</t>
+          <t>Photonic Crystal and Fiber Optics</t>
         </is>
       </c>
       <c r="B404">
@@ -4402,7 +4402,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>Quantum Computing Algorithms and Architecture</t>
+          <t>Photonic and Optical Devices</t>
         </is>
       </c>
       <c r="B405">
@@ -4412,7 +4412,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>Quantum-Dot Cellular Automata</t>
+          <t>Photoreceptor and optogenetics research</t>
         </is>
       </c>
       <c r="B406">
@@ -4422,7 +4422,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>Rabies epidemiology and control</t>
+          <t>Physiological and biochemical adaptations</t>
         </is>
       </c>
       <c r="B407">
@@ -4432,7 +4432,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>Rangeland and Wildlife Management</t>
+          <t>Phytochemicals and Medicinal Plants</t>
         </is>
       </c>
       <c r="B408">
@@ -4442,7 +4442,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>Remote Sensing and LiDAR Applications</t>
+          <t>Planetary Science and Exploration</t>
         </is>
       </c>
       <c r="B409">
@@ -4452,7 +4452,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>Renewable Energy, Sustainability and the Environment</t>
+          <t>Plant Reproductive Biology</t>
         </is>
       </c>
       <c r="B410">
@@ -4462,7 +4462,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>Reproductive Health and Technologies</t>
+          <t>Power System Optimization and Stability</t>
         </is>
       </c>
       <c r="B411">
@@ -4472,7 +4472,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>Reproductive System and Pregnancy</t>
+          <t>Problem and Project Based Learning</t>
         </is>
       </c>
       <c r="B412">
@@ -4482,7 +4482,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>Retinoids in leukemia and cellular processes</t>
+          <t>Prostate Cancer Diagnosis and Treatment</t>
         </is>
       </c>
       <c r="B413">
@@ -4492,7 +4492,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>Rheumatology</t>
+          <t>Protein Tyrosine Phosphatases</t>
         </is>
       </c>
       <c r="B414">
@@ -4502,7 +4502,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>Safety, Risk, Reliability and Quality</t>
+          <t>Psychological Well-being and Life Satisfaction</t>
         </is>
       </c>
       <c r="B415">
@@ -4512,7 +4512,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>Schizophrenia research and treatment</t>
+          <t>Quantum Chromodynamics and Particle Interactions</t>
         </is>
       </c>
       <c r="B416">
@@ -4522,7 +4522,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>Science Education and Pedagogy</t>
+          <t>Quantum Computing Algorithms and Architecture</t>
         </is>
       </c>
       <c r="B417">
@@ -4532,7 +4532,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>Scientific Research and Discoveries</t>
+          <t>Quantum Information and Cryptography</t>
         </is>
       </c>
       <c r="B418">
@@ -4542,7 +4542,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>Scoliosis diagnosis and treatment</t>
+          <t>Quantum Mechanics and Non-Hermitian Physics</t>
         </is>
       </c>
       <c r="B419">
@@ -4552,7 +4552,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>Sensory Systems</t>
+          <t>Quantum-Dot Cellular Automata</t>
         </is>
       </c>
       <c r="B420">
@@ -4562,7 +4562,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>Service and Product Innovation</t>
+          <t>RNA Interference and Gene Delivery</t>
         </is>
       </c>
       <c r="B421">
@@ -4572,7 +4572,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>Sex work and related issues</t>
+          <t>RNA and protein synthesis mechanisms</t>
         </is>
       </c>
       <c r="B422">
@@ -4582,7 +4582,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>Sexuality, Behavior, and Technology</t>
+          <t>RNA modifications and cancer</t>
         </is>
       </c>
       <c r="B423">
@@ -4592,7 +4592,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>Sleep and Work-Related Fatigue</t>
+          <t>Radical Photochemical Reactions</t>
         </is>
       </c>
       <c r="B424">
@@ -4602,7 +4602,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>Solar Radiation and Photovoltaics</t>
+          <t>Recycling and Waste Management Techniques</t>
         </is>
       </c>
       <c r="B425">
@@ -4612,7 +4612,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>Solid State Laser Technologies</t>
+          <t>Rehabilitation</t>
         </is>
       </c>
       <c r="B426">
@@ -4622,7 +4622,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>Solid-state spectroscopy and crystallography</t>
+          <t>Reliability and Maintenance Optimization</t>
         </is>
       </c>
       <c r="B427">
@@ -4632,7 +4632,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>Spacecraft Design and Technology</t>
+          <t>Remote Sensing in Agriculture</t>
         </is>
       </c>
       <c r="B428">
@@ -4642,7 +4642,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>Spacecraft and Cryogenic Technologies</t>
+          <t>Renewable Energy, Sustainability and the Environment</t>
         </is>
       </c>
       <c r="B429">
@@ -4652,7 +4652,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>Spectral Theory in Mathematical Physics</t>
+          <t>Respiratory Support and Mechanisms</t>
         </is>
       </c>
       <c r="B430">
@@ -4662,7 +4662,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>Spectroscopy and Laser Applications</t>
+          <t>Retinal Imaging and Analysis</t>
         </is>
       </c>
       <c r="B431">
@@ -4672,7 +4672,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>Spectroscopy and Quantum Chemical Studies</t>
+          <t>Rock Mechanics and Modeling</t>
         </is>
       </c>
       <c r="B432">
@@ -4682,7 +4682,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>Speech and Hearing</t>
+          <t>SARS-CoV-2 and COVID-19 Research</t>
         </is>
       </c>
       <c r="B433">
@@ -4692,7 +4692,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>Spinal Dysraphism and Malformations</t>
+          <t>SARS-CoV-2 detection and testing</t>
         </is>
       </c>
       <c r="B434">
@@ -4702,7 +4702,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>Spinal Fractures and Fixation Techniques</t>
+          <t>Safety, Risk, Reliability and Quality</t>
         </is>
       </c>
       <c r="B435">
@@ -4712,7 +4712,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>Strategy and Management</t>
+          <t>Salmonella and Campylobacter epidemiology</t>
         </is>
       </c>
       <c r="B436">
@@ -4722,7 +4722,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>Streptococcal Infections and Treatments</t>
+          <t>Seaweed-derived Bioactive Compounds</t>
         </is>
       </c>
       <c r="B437">
@@ -4732,7 +4732,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>Strong Light-Matter Interactions</t>
+          <t>Skin Protection and Aging</t>
         </is>
       </c>
       <c r="B438">
@@ -4742,7 +4742,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>Substance Abuse Treatment and Outcomes</t>
+          <t>Sleep and Work-Related Fatigue</t>
         </is>
       </c>
       <c r="B439">
@@ -4752,7 +4752,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>Surfaces, Coatings and Films</t>
+          <t>Smart Grid Security and Resilience</t>
         </is>
       </c>
       <c r="B440">
@@ -4762,7 +4762,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>Surgical site infection prevention</t>
+          <t>Social and Intergroup Psychology</t>
         </is>
       </c>
       <c r="B441">
@@ -4772,7 +4772,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>Synthesis and Catalytic Reactions</t>
+          <t>Software</t>
         </is>
       </c>
       <c r="B442">
@@ -4782,7 +4782,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>Synthesis and biological activity</t>
+          <t>Software Reliability and Analysis Research</t>
         </is>
       </c>
       <c r="B443">
@@ -4792,7 +4792,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>Systemic Sclerosis and Related Diseases</t>
+          <t>Software-Defined Networks and 5G</t>
         </is>
       </c>
       <c r="B444">
@@ -4802,7 +4802,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>Technology Adoption and User Behaviour</t>
+          <t>Solar Radiation and Photovoltaics</t>
         </is>
       </c>
       <c r="B445">
@@ -4812,7 +4812,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>Toxicology</t>
+          <t>Spacecraft Dynamics and Control</t>
         </is>
       </c>
       <c r="B446">
@@ -4822,7 +4822,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>Tree Root and Stability Studies</t>
+          <t>Spacecraft and Cryogenic Technologies</t>
         </is>
       </c>
       <c r="B447">
@@ -4832,7 +4832,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>Tuberculosis Research and Epidemiology</t>
+          <t>Spaceflight effects on biology</t>
         </is>
       </c>
       <c r="B448">
@@ -4842,7 +4842,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>Urban Studies</t>
+          <t>Spam and Phishing Detection</t>
         </is>
       </c>
       <c r="B449">
@@ -4852,7 +4852,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>Urban and Rural Development Challenges</t>
+          <t>Spectral Theory in Mathematical Physics</t>
         </is>
       </c>
       <c r="B450">
@@ -4862,7 +4862,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>Uterine Myomas and Treatments</t>
+          <t>Spectroscopy and Quantum Chemical Studies</t>
         </is>
       </c>
       <c r="B451">
@@ -4872,7 +4872,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>Vehicle License Plate Recognition</t>
+          <t>Statistical Distribution Estimation and Applications</t>
         </is>
       </c>
       <c r="B452">
@@ -4882,7 +4882,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>Venomous Animal Envenomation and Studies</t>
+          <t>Statistical and Nonlinear Physics</t>
         </is>
       </c>
       <c r="B453">
@@ -4892,7 +4892,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>Venous Thromboembolism Diagnosis and Management</t>
+          <t>Statistics and Probability</t>
         </is>
       </c>
       <c r="B454">
@@ -4902,7 +4902,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>Virology</t>
+          <t>Stock Market Forecasting Methods</t>
         </is>
       </c>
       <c r="B455">
@@ -4912,7 +4912,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>Vitamin D Research Studies</t>
+          <t>Stroke Rehabilitation and Recovery</t>
         </is>
       </c>
       <c r="B456">
@@ -4922,7 +4922,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>Voice and Speech Disorders</t>
+          <t>Structural Health Monitoring Techniques</t>
         </is>
       </c>
       <c r="B457">
@@ -4932,7 +4932,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>Wastewater Treatment and Reuse</t>
+          <t>Sulfur-Based Synthesis Techniques</t>
         </is>
       </c>
       <c r="B458">
@@ -4942,7 +4942,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>Wildlife Ecology and Conservation</t>
+          <t>Tactile and Sensory Interactions</t>
         </is>
       </c>
       <c r="B459">
@@ -4952,7 +4952,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>Zebrafish Biomedical Research Applications</t>
+          <t>Tardigrade Biology and Ecology</t>
         </is>
       </c>
       <c r="B460">
@@ -4962,10 +4962,150 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>earthquake and tectonic studies</t>
+          <t>Time Series Analysis and Forecasting</t>
         </is>
       </c>
       <c r="B461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>Trauma and Emergency Care Studies</t>
+        </is>
+      </c>
+      <c r="B462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>Tree-ring climate responses</t>
+        </is>
+      </c>
+      <c r="B463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>Tribology and Wear Analysis</t>
+        </is>
+      </c>
+      <c r="B464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>Urinary Tract Infections Management</t>
+        </is>
+      </c>
+      <c r="B465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>User Authentication and Security Systems</t>
+        </is>
+      </c>
+      <c r="B466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>Vagus Nerve Stimulation Research</t>
+        </is>
+      </c>
+      <c r="B467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>Venous Thromboembolism Diagnosis and Management</t>
+        </is>
+      </c>
+      <c r="B468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>Vibrio bacteria research studies</t>
+        </is>
+      </c>
+      <c r="B469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>Virology</t>
+        </is>
+      </c>
+      <c r="B470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>Water Quality Monitoring Technologies</t>
+        </is>
+      </c>
+      <c r="B471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>Welding Techniques and Residual Stresses</t>
+        </is>
+      </c>
+      <c r="B472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>Wildlife Ecology and Conservation</t>
+        </is>
+      </c>
+      <c r="B473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>biodegradable polymer synthesis and properties</t>
+        </is>
+      </c>
+      <c r="B474">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>graph theory and CDMA systems</t>
+        </is>
+      </c>
+      <c r="B475">
         <v>1</v>
       </c>
     </row>

</xml_diff>